<commit_message>
porcentagem de cada metas adicionado
</commit_message>
<xml_diff>
--- a/metas.xlsx
+++ b/metas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guigu\OneDrive\Área de Trabalho\AureaBot\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guigu\OneDrive\Área de Trabalho\AureaBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E1AE2-40E8-47E4-98E4-BD02BB27B821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611F76EC-2990-4D22-A011-004F7801BBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{73FC0B26-8210-4731-AB5C-6D60C659D95E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FC0B26-8210-4731-AB5C-6D60C659D95E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -48,12 +48,6 @@
     <t>Projetos</t>
   </si>
   <si>
-    <t>53k</t>
-  </si>
-  <si>
-    <t>24.9k</t>
-  </si>
-  <si>
     <t>NPS</t>
   </si>
   <si>
@@ -67,13 +61,32 @@
   </si>
   <si>
     <t>Participacao_em_eventos</t>
+  </si>
+  <si>
+    <t>Porcentagem</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,14 +112,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,23 +451,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D3FD3-1844-4F5C-BB3A-D01F4FAA5A4A}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -442,71 +477,115 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>23</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>65</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>75</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>80</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="4">
+        <v>24.9</v>
+      </c>
+      <c r="C3" s="1">
         <v>16</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>100</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>80</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>80</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6">
+        <f>((B3*100)/B2)</f>
+        <v>46.981132075471699</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:H4" si="0">((C3*100)/C2)</f>
+        <v>69.565217391304344</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <v>100</v>
+      </c>
+      <c r="F4" s="2">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I4" s="5">
+        <f>(SUM(B4:H4)/7)</f>
+        <v>75.220907066682301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quadro de lideranças adicionado
</commit_message>
<xml_diff>
--- a/metas.xlsx
+++ b/metas.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guigu\OneDrive\Área de Trabalho\AureaBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611F76EC-2990-4D22-A011-004F7801BBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1780B179-FBE2-4077-8DF9-19279823B588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FC0B26-8210-4731-AB5C-6D60C659D95E}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{73FC0B26-8210-4731-AB5C-6D60C659D95E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Metas</t>
   </si>
@@ -67,6 +69,99 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Diretores</t>
+  </si>
+  <si>
+    <t>Presidente</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Comercial</t>
+  </si>
+  <si>
+    <t>Gente_e_Gestao</t>
+  </si>
+  <si>
+    <t>Daniel Fonseca</t>
+  </si>
+  <si>
+    <t>Aline Maia</t>
+  </si>
+  <si>
+    <t>Vinius Santi</t>
+  </si>
+  <si>
+    <t>Jardel Salles</t>
+  </si>
+  <si>
+    <t>Kleber Azeredo</t>
+  </si>
+  <si>
+    <t>Coordenadores</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>Eletr</t>
+  </si>
+  <si>
+    <t>Autom</t>
+  </si>
+  <si>
+    <t>Endo</t>
+  </si>
+  <si>
+    <t>Inbound</t>
+  </si>
+  <si>
+    <t>PosV</t>
+  </si>
+  <si>
+    <t>Vendas</t>
+  </si>
+  <si>
+    <t>Gente</t>
+  </si>
+  <si>
+    <t>Gestao</t>
+  </si>
+  <si>
+    <t>Rayssa Alves</t>
+  </si>
+  <si>
+    <t>Higor Brandão</t>
+  </si>
+  <si>
+    <t>Laura Barros</t>
+  </si>
+  <si>
+    <t>Diogo Ribeiro</t>
+  </si>
+  <si>
+    <t>Guilherme Barreto</t>
+  </si>
+  <si>
+    <t>Micaella Barcellos</t>
+  </si>
+  <si>
+    <t>João Carvalho</t>
+  </si>
+  <si>
+    <t>Matheus Henrique</t>
+  </si>
+  <si>
+    <t>Talita Silva</t>
+  </si>
+  <si>
+    <t>Giana Bastos</t>
+  </si>
+  <si>
+    <t>ArqEUrb</t>
   </si>
 </sst>
 </file>
@@ -76,8 +171,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -122,13 +217,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -453,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D3FD3-1844-4F5C-BB3A-D01F4FAA5A4A}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -592,4 +687,158 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB8A45B-6578-4D00-81DC-C6286FF2A9B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC12A05B-6148-443C-BD60-A0AC19AD36F3}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>